<commit_message>
Expense Req latest changes
</commit_message>
<xml_diff>
--- a/TestData/TMTT0017340_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsRequestor.xlsx
+++ b/TestData/TMTT0017340_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsRequestor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HL\SalesForce_Project\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBE6DD6-532B-408F-BB4A-6F2A727BCDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A5B411-B445-41A9-B4BE-732FF8057CEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="6804" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpenseRequest" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>LOB</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>CF_Event123</t>
-  </si>
-  <si>
-    <t>Amanda Donovan</t>
   </si>
   <si>
     <t>Emre Abale</t>
@@ -491,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -548,22 +545,22 @@
         <v>23</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="O1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
@@ -571,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>25</v>
@@ -601,19 +598,19 @@
         <v>22</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
         <v>33</v>
       </c>
-      <c r="N2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" t="s">
-        <v>34</v>
-      </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q2" t="s">
         <v>22</v>
@@ -627,10 +624,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,16 +642,11 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CF Expense Request changes - 5th Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTT0017340_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsRequestor.xlsx
+++ b/TestData/TMTT0017340_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsRequestor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A37252-E381-4954-BDBF-E19983A7BD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9941B54-420C-4630-8D4F-CEAD32E47F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>LOBErrorMsg</t>
   </si>
   <si>
-    <t>Complete this field.</t>
-  </si>
-  <si>
     <t>DifferentReqErrorMsg</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>PFG Golf Event</t>
+  </si>
+  <si>
+    <t>Complete this field</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,7 +504,7 @@
     <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21.6640625" customWidth="1"/>
     <col min="15" max="15" width="31.88671875" customWidth="1"/>
@@ -548,19 +548,19 @@
         <v>25</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="O1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
@@ -568,13 +568,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
@@ -598,19 +598,19 @@
         <v>22</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
         <v>30</v>
       </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
-      </c>
       <c r="P2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q2" t="s">
         <v>22</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>